<commit_message>
Fikset beregning for admittanser og gjort eksporten til excel finere.
</commit_message>
<xml_diff>
--- a/Linjeimpedanser_uten_avrunding.xlsx
+++ b/Linjeimpedanser_uten_avrunding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arntzen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCA213B-44B3-3E44-B04B-34E72F64EEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D797F5EB-F1EB-4649-89EA-8F6F37433CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Linje</t>
   </si>
@@ -31,18 +31,24 @@
     <t>Impedans (p.u.)</t>
   </si>
   <si>
+    <t>Admittans (p.u.)</t>
+  </si>
+  <si>
     <t>Kapasitans (nF)</t>
   </si>
   <si>
     <t>1-2</t>
   </si>
   <si>
-    <t>(0.916+9.847j)</t>
+    <t>(0.9159999999999999+9.847j)</t>
   </si>
   <si>
     <t>(0.010177777777777777+0.10941111111111111j)</t>
   </si>
   <si>
+    <t>(0.8429235398105763-9.061428052963697j)</t>
+  </si>
+  <si>
     <t>2-3</t>
   </si>
   <si>
@@ -52,6 +58,9 @@
     <t>(0.008355555555555555+0.08982222222222222j)</t>
   </si>
   <si>
+    <t>(1.0267526096628827-11.03759055387599j)</t>
+  </si>
+  <si>
     <t>3-4</t>
   </si>
   <si>
@@ -61,6 +70,9 @@
     <t>(0.021244444444444444+0.22837777777777776j)</t>
   </si>
   <si>
+    <t>(0.4038273862272426-4.341144401942858j)</t>
+  </si>
+  <si>
     <t>4-5</t>
   </si>
   <si>
@@ -70,15 +82,21 @@
     <t>(0.004033333333333333+0.044366666666666665j)</t>
   </si>
   <si>
+    <t>(2.0322449532583664-22.35469448584203j)</t>
+  </si>
+  <si>
     <t>5-6</t>
   </si>
   <si>
-    <t>(1.424+22.784j)</t>
+    <t>(1.4240000000000002+22.784000000000002j)</t>
   </si>
   <si>
     <t>(0.015822222222222224+0.2531555555555556j)</t>
   </si>
   <si>
+    <t>(0.24592314082105537-3.934770253136886j)</t>
+  </si>
+  <si>
     <t>6-7</t>
   </si>
   <si>
@@ -88,15 +106,21 @@
     <t>(0.01208888888888889+0.19342222222222225j)</t>
   </si>
   <si>
+    <t>(0.3218699931334401-5.149919890135042j)</t>
+  </si>
+  <si>
     <t>7-8</t>
   </si>
   <si>
-    <t>(1.976+21.242j)</t>
+    <t>(1.976+21.241999999999997j)</t>
   </si>
   <si>
     <t>(0.021955555555555555+0.2360222222222222j)</t>
   </si>
   <si>
+    <t>(0.3907479567138098-4.200540534673455j)</t>
+  </si>
+  <si>
     <t>1-8</t>
   </si>
   <si>
@@ -106,6 +130,9 @@
     <t>(0.04702222222222223+0.5054888888888889j)</t>
   </si>
   <si>
+    <t>(0.182447533664104-1.9613109868891176j)</t>
+  </si>
+  <si>
     <t>1-6</t>
   </si>
   <si>
@@ -113,6 +140,9 @@
   </si>
   <si>
     <t>(0.05186666666666667+0.5575666666666667j)</t>
+  </si>
+  <si>
+    <t>(0.16540659007422623-1.7781208432979319j)</t>
   </si>
 </sst>
 </file>
@@ -131,6 +161,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -475,20 +506,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,130 +533,160 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
         <v>199.23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>163.56</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
         <v>415.86</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
         <v>136.72999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
         <v>811.68000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7">
         <v>620.16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8">
         <v>429.78</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9">
         <v>920.45999999999992</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10">
         <v>1015.29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fått riktig verdier for linjeadmittansene.
</commit_message>
<xml_diff>
--- a/Linjeimpedanser_uten_avrunding.xlsx
+++ b/Linjeimpedanser_uten_avrunding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arntzen/Desktop/IELET2118---Prosjekt-Lastflytanalyse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39B090C-CB92-0C45-821E-767EB5B8FCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9770AA80-56A7-EB48-B7CC-F02784D9BDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Linje</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Kapasitans (nF)</t>
   </si>
   <si>
+    <t>Shunt Impedans (ohm)</t>
+  </si>
+  <si>
     <t>Shunt Admittans (ohm)</t>
   </si>
   <si>
@@ -58,13 +61,16 @@
     <t>(0.8429235398105763-9.061428052963697j)</t>
   </si>
   <si>
-    <t>62589.95043746944j</t>
-  </si>
-  <si>
-    <t>695.4438937496604j</t>
-  </si>
-  <si>
-    <t>347.7219468748302j</t>
+    <t>-15977.005781448112j</t>
+  </si>
+  <si>
+    <t>6.258995043746944e-05j</t>
+  </si>
+  <si>
+    <t>0.005633095539372249j</t>
+  </si>
+  <si>
+    <t>0.0028165477696861247j</t>
   </si>
   <si>
     <t>2-3</t>
@@ -79,13 +85,16 @@
     <t>(1.0267526096628827-11.03759055387599j)</t>
   </si>
   <si>
-    <t>51383.88944211466j</t>
-  </si>
-  <si>
-    <t>570.9321049123852j</t>
-  </si>
-  <si>
-    <t>285.4660524561926j</t>
+    <t>-19461.352786976684j</t>
+  </si>
+  <si>
+    <t>5.1383889442114665e-05j</t>
+  </si>
+  <si>
+    <t>0.00462455004979032j</t>
+  </si>
+  <si>
+    <t>0.00231227502489516j</t>
   </si>
   <si>
     <t>3-4</t>
@@ -100,13 +109,16 @@
     <t>(0.4038273862272426-4.341144401942858j)</t>
   </si>
   <si>
-    <t>130646.27209218513j</t>
-  </si>
-  <si>
-    <t>1451.6252454687237j</t>
-  </si>
-  <si>
-    <t>725.8126227343619j</t>
+    <t>-7654.255907848572j</t>
+  </si>
+  <si>
+    <t>0.00013064627209218512j</t>
+  </si>
+  <si>
+    <t>0.011758164488296662j</t>
+  </si>
+  <si>
+    <t>0.005879082244148331j</t>
   </si>
   <si>
     <t>4-5</t>
@@ -121,13 +133,16 @@
     <t>(2.0322449532583664-22.35469448584203j)</t>
   </si>
   <si>
-    <t>42954.99635253325j</t>
-  </si>
-  <si>
-    <t>477.27773725036946j</t>
-  </si>
-  <si>
-    <t>238.63886862518473j</t>
+    <t>-23280.17890615012j</t>
+  </si>
+  <si>
+    <t>4.2954996352533256e-05j</t>
+  </si>
+  <si>
+    <t>0.003865949671727993j</t>
+  </si>
+  <si>
+    <t>0.0019329748358639966j</t>
   </si>
   <si>
     <t>5-6</t>
@@ -142,13 +157,16 @@
     <t>(0.24592314082105537-3.934770253136886j)</t>
   </si>
   <si>
-    <t>254996.79250657637j</t>
-  </si>
-  <si>
-    <t>2833.297694517515j</t>
-  </si>
-  <si>
-    <t>1416.6488472587575j</t>
+    <t>-3921.6179551521614j</t>
+  </si>
+  <si>
+    <t>0.0002549967925065764j</t>
+  </si>
+  <si>
+    <t>0.022949711325591874j</t>
+  </si>
+  <si>
+    <t>0.011474855662795937j</t>
   </si>
   <si>
     <t>6-7</t>
@@ -163,13 +181,16 @@
     <t>(0.3218699931334401-5.149919890135042j)</t>
   </si>
   <si>
-    <t>194829.0100050246j</t>
-  </si>
-  <si>
-    <t>2164.7667778336067j</t>
-  </si>
-  <si>
-    <t>1082.3833889168034j</t>
+    <t>-5132.7058530668j</t>
+  </si>
+  <si>
+    <t>0.0001948290100050246j</t>
+  </si>
+  <si>
+    <t>0.017534610900452215j</t>
+  </si>
+  <si>
+    <t>0.008767305450226108j</t>
   </si>
   <si>
     <t>7-8</t>
@@ -184,13 +205,16 @@
     <t>(0.3907479567138098-4.200540534673455j)</t>
   </si>
   <si>
-    <t>135019.36906598211j</t>
-  </si>
-  <si>
-    <t>1500.2152118442457j</t>
-  </si>
-  <si>
-    <t>750.1076059221228j</t>
+    <t>-7406.34478532716j</t>
+  </si>
+  <si>
+    <t>0.00013501936906598212j</t>
+  </si>
+  <si>
+    <t>0.012151743215938392j</t>
+  </si>
+  <si>
+    <t>0.006075871607969196j</t>
   </si>
   <si>
     <t>1-8</t>
@@ -205,13 +229,16 @@
     <t>(0.182447533664104-1.9613109868891176j)</t>
   </si>
   <si>
-    <t>289171.0373923261j</t>
-  </si>
-  <si>
-    <t>3213.011526581401j</t>
-  </si>
-  <si>
-    <t>1606.5057632907005j</t>
+    <t>-3458.160986721755j</t>
+  </si>
+  <si>
+    <t>0.0002891710373923261j</t>
+  </si>
+  <si>
+    <t>0.02602539336530935j</t>
+  </si>
+  <si>
+    <t>0.013012696682654675j</t>
   </si>
   <si>
     <t>1-6</t>
@@ -226,13 +253,16 @@
     <t>(0.16540659007422623-1.7781208432979319j)</t>
   </si>
   <si>
-    <t>318962.7605263181j</t>
-  </si>
-  <si>
-    <t>3544.0306725146456j</t>
-  </si>
-  <si>
-    <t>1772.0153362573228j</t>
+    <t>-3135.162231321008j</t>
+  </si>
+  <si>
+    <t>0.00031896276052631814j</t>
+  </si>
+  <si>
+    <t>0.028706648447368633j</t>
+  </si>
+  <si>
+    <t>0.014353324223684316j</t>
   </si>
 </sst>
 </file>
@@ -595,25 +625,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="41.33203125" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" customWidth="1"/>
-    <col min="4" max="4" width="42" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="44.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.5" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" customWidth="1"/>
+    <col min="8" max="8" width="23.5" customWidth="1"/>
+    <col min="9" max="9" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,239 +668,269 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>199.23</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>163.56</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>415.86</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E5">
         <v>136.72999999999999</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E6">
         <v>811.68000000000006</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E7">
         <v>620.16</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E8">
         <v>429.78</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="I8" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E9">
         <v>920.45999999999992</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+      <c r="I9" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E10">
         <v>1015.29</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>79</v>
+      </c>
+      <c r="I10" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lagt til prosjektfiler fra BB, og begynt å fylle inn systemdata - basecase
</commit_message>
<xml_diff>
--- a/Linjeimpedanser_uten_avrunding.xlsx
+++ b/Linjeimpedanser_uten_avrunding.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arntzen/Desktop/IELET2118---Prosjekt-Lastflytanalyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9770AA80-56A7-EB48-B7CC-F02784D9BDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF187D2-5635-41D4-9E36-0140FEBEF64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Base Case" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -49,9 +62,6 @@
     <t>Shunt Admittans (p.u.) half</t>
   </si>
   <si>
-    <t>1-2</t>
-  </si>
-  <si>
     <t>(0.9159999999999999+9.847j)</t>
   </si>
   <si>
@@ -73,9 +83,6 @@
     <t>0.0028165477696861247j</t>
   </si>
   <si>
-    <t>2-3</t>
-  </si>
-  <si>
     <t>(0.752+8.084j)</t>
   </si>
   <si>
@@ -97,9 +104,6 @@
     <t>0.00231227502489516j</t>
   </si>
   <si>
-    <t>3-4</t>
-  </si>
-  <si>
     <t>(1.912+20.554j)</t>
   </si>
   <si>
@@ -121,9 +125,6 @@
     <t>0.005879082244148331j</t>
   </si>
   <si>
-    <t>4-5</t>
-  </si>
-  <si>
     <t>(0.363+3.993j)</t>
   </si>
   <si>
@@ -145,9 +146,6 @@
     <t>0.0019329748358639966j</t>
   </si>
   <si>
-    <t>5-6</t>
-  </si>
-  <si>
     <t>(1.4240000000000002+22.784000000000002j)</t>
   </si>
   <si>
@@ -169,9 +167,6 @@
     <t>0.011474855662795937j</t>
   </si>
   <si>
-    <t>6-7</t>
-  </si>
-  <si>
     <t>(1.088+17.408j)</t>
   </si>
   <si>
@@ -193,9 +188,6 @@
     <t>0.008767305450226108j</t>
   </si>
   <si>
-    <t>7-8</t>
-  </si>
-  <si>
     <t>(1.976+21.241999999999997j)</t>
   </si>
   <si>
@@ -217,9 +209,6 @@
     <t>0.006075871607969196j</t>
   </si>
   <si>
-    <t>1-8</t>
-  </si>
-  <si>
     <t>(4.232+45.494j)</t>
   </si>
   <si>
@@ -241,9 +230,6 @@
     <t>0.013012696682654675j</t>
   </si>
   <si>
-    <t>1-6</t>
-  </si>
-  <si>
     <t>(4.668+50.181j)</t>
   </si>
   <si>
@@ -263,6 +249,33 @@
   </si>
   <si>
     <t>0.014353324223684316j</t>
+  </si>
+  <si>
+    <t>1 — 2</t>
+  </si>
+  <si>
+    <t>2 — 3</t>
+  </si>
+  <si>
+    <t>3 — 4</t>
+  </si>
+  <si>
+    <t>4 — 5</t>
+  </si>
+  <si>
+    <t>5 — 6</t>
+  </si>
+  <si>
+    <t>6 — 7</t>
+  </si>
+  <si>
+    <t>7 — 8</t>
+  </si>
+  <si>
+    <t>1 — 8</t>
+  </si>
+  <si>
+    <t>1 — 6</t>
   </si>
 </sst>
 </file>
@@ -318,10 +331,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,23 +643,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.83203125" customWidth="1"/>
-    <col min="4" max="4" width="40.5" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="7" width="27.83203125" customWidth="1"/>
-    <col min="8" max="8" width="23.5" customWidth="1"/>
-    <col min="9" max="9" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,265 +688,265 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
       </c>
       <c r="E2">
         <v>199.23</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
       </c>
       <c r="E3">
         <v>163.56</v>
       </c>
       <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
       </c>
       <c r="E4">
         <v>415.86</v>
       </c>
       <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="I4" t="s">
+      <c r="D5" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
       </c>
       <c r="E5">
         <v>136.72999999999999</v>
       </c>
       <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="G5" t="s">
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="H5" t="s">
+      <c r="D6" t="s">
         <v>39</v>
-      </c>
-      <c r="I5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
       </c>
       <c r="E6">
         <v>811.68000000000006</v>
       </c>
       <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="G6" t="s">
+      <c r="D7" t="s">
         <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
       </c>
       <c r="E7">
         <v>620.16</v>
       </c>
       <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
         <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
       </c>
       <c r="E8">
         <v>429.78</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>65</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E9">
         <v>920.45999999999992</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>73</v>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <v>1015.29</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>